<commit_message>
chore: updated city order
</commit_message>
<xml_diff>
--- a/1-data/1-research/cities.latest.xlsx
+++ b/1-data/1-research/cities.latest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="292">
   <si>
     <t>city_name</t>
   </si>
@@ -26,6 +26,12 @@
   </si>
   <si>
     <t>priority</t>
+  </si>
+  <si>
+    <t>Trnava</t>
+  </si>
+  <si>
+    <t>SVK</t>
   </si>
   <si>
     <t>Amsterdam</t>
@@ -948,7 +954,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -961,9 +967,6 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1279,13 +1282,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1299,43 +1302,43 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="2">
+        <v>3101</v>
+      </c>
+      <c r="D2" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4">
         <v>2167</v>
       </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2226</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C4" s="2">
-        <v>2205</v>
+        <v>2226</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -1343,13 +1346,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2">
-        <v>2269</v>
+        <v>2205</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -1357,13 +1360,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2">
-        <v>2138</v>
+        <v>2269</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -1371,13 +1374,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2">
-        <v>2220</v>
+        <v>2138</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -1385,13 +1388,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
-        <v>2219</v>
+        <v>2220</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -1399,13 +1402,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2">
-        <v>2123</v>
+        <v>2219</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -1413,13 +1416,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2">
-        <v>2183</v>
+        <v>2123</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
@@ -1427,13 +1430,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2">
-        <v>2180</v>
+        <v>2183</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
@@ -1441,10 +1444,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2">
         <v>2181</v>
@@ -1455,10 +1458,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C13" s="2">
         <v>2194</v>
@@ -1469,10 +1472,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2">
         <v>1105</v>
@@ -1483,10 +1486,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C15" s="2">
         <v>12977</v>
@@ -1497,10 +1500,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2">
         <v>13023</v>
@@ -1511,10 +1514,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C17" s="2">
         <v>11640</v>
@@ -1525,10 +1528,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C18" s="2">
         <v>13043</v>
@@ -1539,52 +1542,52 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2">
         <v>3000</v>
       </c>
       <c r="D19" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C20" s="2">
         <v>3027</v>
       </c>
       <c r="D20" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C21" s="2">
         <v>2135</v>
       </c>
       <c r="D21" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C22" s="2">
         <v>1361</v>
@@ -1595,10 +1598,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C23" s="2">
         <v>1420</v>
@@ -1609,10 +1612,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C24" s="2">
         <v>362</v>
@@ -1623,10 +1626,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C25" s="2">
         <v>1017</v>
@@ -1637,10 +1640,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="C26" s="2">
         <v>875</v>
@@ -1651,24 +1654,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C27" s="2">
         <v>2384</v>
       </c>
       <c r="D27" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C28" s="2">
         <v>906</v>
@@ -1679,10 +1682,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C29" s="2">
         <v>931</v>
@@ -1693,10 +1696,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C30" s="2">
         <v>621</v>
@@ -1705,222 +1708,222 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C31" s="2">
         <v>2927</v>
       </c>
       <c r="D31" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C32" s="2">
         <v>2851</v>
       </c>
       <c r="D32" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C33" s="2">
         <v>2531</v>
       </c>
       <c r="D33" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C34" s="2">
         <v>2518</v>
       </c>
       <c r="D34" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
       <c r="A35" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C35" s="2">
         <v>2749</v>
       </c>
       <c r="D35" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
       <c r="A36" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C36" s="2">
         <v>2051</v>
       </c>
       <c r="D36" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
       <c r="A37" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C37" s="2">
         <v>1701</v>
       </c>
       <c r="D37" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
       <c r="A38" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C38" s="2">
         <v>3255</v>
       </c>
       <c r="D38" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
       <c r="A39" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C39" s="2">
         <v>3244</v>
       </c>
       <c r="D39" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18">
       <c r="A40" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C40" s="2">
         <v>2228</v>
       </c>
       <c r="D40" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18">
       <c r="A41" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C41" s="2">
         <v>2046</v>
       </c>
       <c r="D41" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18">
       <c r="A42" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C42" s="2">
         <v>1800</v>
       </c>
       <c r="D42" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18">
       <c r="A43" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C43" s="2">
         <v>1912</v>
       </c>
       <c r="D43" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18">
       <c r="A44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C44" s="2">
         <v>1874</v>
       </c>
       <c r="D44" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18">
       <c r="A45" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C45" s="2">
         <v>3193</v>
       </c>
       <c r="D45" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18">
       <c r="A46" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C46" s="2">
         <v>6845</v>
@@ -1931,10 +1934,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18">
       <c r="A47" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C47" s="2">
         <v>6955</v>
@@ -1945,52 +1948,52 @@
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18">
       <c r="A48" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C48" s="2">
         <v>1656</v>
       </c>
       <c r="D48" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18">
       <c r="A49" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C49" s="2">
         <v>2253</v>
       </c>
       <c r="D49" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18">
       <c r="A50" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C50" s="2">
         <v>3269</v>
       </c>
       <c r="D50" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18">
       <c r="A51" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C51" s="2">
         <v>154</v>
@@ -2001,10 +2004,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18">
       <c r="A52" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C52" s="2">
         <v>11139</v>
@@ -2015,24 +2018,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18">
       <c r="A53" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C53" s="2">
         <v>2493</v>
       </c>
       <c r="D53" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18">
       <c r="A54" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C54" s="2">
         <v>13129</v>
@@ -2043,10 +2046,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18">
       <c r="A55" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C55" s="2">
         <v>13121</v>
@@ -2057,66 +2060,66 @@
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18">
       <c r="A56" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C56" s="2">
         <v>3216</v>
       </c>
       <c r="D56" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18">
       <c r="A57" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C57" s="2">
         <v>1551</v>
       </c>
       <c r="D57" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18">
       <c r="A58" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C58" s="2">
         <v>2682</v>
       </c>
       <c r="D58" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18">
       <c r="A59" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C59" s="2">
         <v>2973</v>
       </c>
       <c r="D59" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18">
       <c r="A60" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C60" s="2">
         <v>634</v>
@@ -2127,10 +2130,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18">
       <c r="A61" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C61" s="2">
         <v>323</v>
@@ -2141,10 +2144,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18">
       <c r="A62" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="C62" s="2">
         <v>315</v>
@@ -2155,10 +2158,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18">
       <c r="A63" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C63" s="2">
         <v>14</v>
@@ -2169,10 +2172,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18">
       <c r="A64" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C64" s="2">
         <v>945</v>
@@ -2183,10 +2186,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18">
       <c r="A65" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C65" s="2">
         <v>898</v>
@@ -2197,10 +2200,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18">
       <c r="A66" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C66" s="2">
         <v>79</v>
@@ -2211,10 +2214,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18">
       <c r="A67" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C67" s="2">
         <v>101</v>
@@ -2225,10 +2228,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18">
       <c r="A68" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C68" s="2">
         <v>1303</v>
@@ -2239,24 +2242,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18">
       <c r="A69" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C69" s="2">
         <v>2083</v>
       </c>
       <c r="D69" s="2">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18">
       <c r="A70" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C70" s="2">
         <v>1117</v>
@@ -2267,10 +2270,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18">
       <c r="A71" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C71" s="2">
         <v>13076</v>
@@ -2281,24 +2284,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18">
       <c r="A72" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C72" s="2">
         <v>2788</v>
       </c>
       <c r="D72" s="2">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18">
       <c r="A73" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C73" s="2">
         <v>2936</v>
@@ -2309,10 +2312,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18">
       <c r="A74" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C74" s="2">
         <v>2885</v>
@@ -2323,10 +2326,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18">
       <c r="A75" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C75" s="2">
         <v>5528</v>
@@ -2337,10 +2340,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18">
       <c r="A76" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C76" s="2">
         <v>2133</v>
@@ -2351,10 +2354,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18">
       <c r="A77" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C77" s="2">
         <v>2112</v>
@@ -2365,10 +2368,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18">
       <c r="A78" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C78" s="2">
         <v>3381</v>
@@ -2379,10 +2382,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18">
       <c r="A79" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C79" s="2">
         <v>3196</v>
@@ -2393,10 +2396,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18">
       <c r="A80" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C80" s="2">
         <v>849</v>
@@ -2407,10 +2410,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18">
       <c r="A81" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C81" s="2">
         <v>940</v>
@@ -2421,10 +2424,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18">
       <c r="A82" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C82" s="2">
         <v>1242</v>
@@ -2435,10 +2438,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18">
       <c r="A83" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C83" s="2">
         <v>1218</v>
@@ -2449,10 +2452,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18">
       <c r="A84" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C84" s="2">
         <v>1115</v>
@@ -2463,10 +2466,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18">
       <c r="A85" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C85" s="2">
         <v>834</v>
@@ -2477,10 +2480,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18">
       <c r="A86" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C86" s="2">
         <v>989</v>
@@ -2491,10 +2494,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18">
       <c r="A87" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C87" s="2">
         <v>187</v>
@@ -2505,10 +2508,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18">
       <c r="A88" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C88" s="2">
         <v>160</v>
@@ -2519,10 +2522,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18">
       <c r="A89" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C89" s="2">
         <v>2392</v>
@@ -2533,10 +2536,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18">
       <c r="A90" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C90" s="2">
         <v>2314</v>
@@ -2547,10 +2550,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18">
       <c r="A91" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C91" s="2">
         <v>2463</v>
@@ -2561,10 +2564,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18">
       <c r="A92" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C92" s="2">
         <v>10687</v>
@@ -2575,10 +2578,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18">
       <c r="A93" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C93" s="2">
         <v>3036</v>
@@ -2589,10 +2592,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18">
       <c r="A94" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C94" s="2">
         <v>3120</v>
@@ -2603,10 +2606,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18">
       <c r="A95" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C95" s="2">
         <v>2245</v>
@@ -2617,10 +2620,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18">
       <c r="A96" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C96" s="2">
         <v>2734</v>
@@ -2631,10 +2634,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18">
       <c r="A97" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C97" s="2">
         <v>2716</v>
@@ -2645,10 +2648,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18">
       <c r="A98" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C98" s="2">
         <v>2432</v>
@@ -2659,10 +2662,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18">
       <c r="A99" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C99" s="2">
         <v>2439</v>
@@ -2673,10 +2676,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18">
       <c r="A100" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C100" s="2">
         <v>2417</v>
@@ -2687,10 +2690,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18">
       <c r="A101" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C101" s="2">
         <v>2641</v>
@@ -2701,10 +2704,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18">
       <c r="A102" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C102" s="2">
         <v>2852</v>
@@ -2715,10 +2718,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18">
       <c r="A103" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C103" s="2">
         <v>2310</v>
@@ -2729,10 +2732,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18">
       <c r="A104" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C104" s="2">
         <v>2549</v>
@@ -2743,10 +2746,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18">
       <c r="A105" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C105" s="2">
         <v>2916</v>
@@ -2757,10 +2760,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18">
       <c r="A106" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C106" s="2">
         <v>2461</v>
@@ -2771,10 +2774,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18">
       <c r="A107" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C107" s="2">
         <v>2276</v>
@@ -2785,10 +2788,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18">
       <c r="A108" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C108" s="2">
         <v>2887</v>
@@ -2799,10 +2802,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18">
       <c r="A109" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C109" s="2">
         <v>2288</v>
@@ -2813,10 +2816,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18">
       <c r="A110" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C110" s="2">
         <v>2713</v>
@@ -2827,10 +2830,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18">
       <c r="A111" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C111" s="2">
         <v>2733</v>
@@ -2841,10 +2844,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18">
       <c r="A112" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C112" s="2">
         <v>2474</v>
@@ -2855,10 +2858,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18">
       <c r="A113" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C113" s="2">
         <v>2445</v>
@@ -2869,10 +2872,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18">
       <c r="A114" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C114" s="2">
         <v>2408</v>
@@ -2883,10 +2886,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18">
       <c r="A115" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C115" s="2">
         <v>2799</v>
@@ -2897,10 +2900,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18">
       <c r="A116" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C116" s="2">
         <v>2942</v>
@@ -2911,10 +2914,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18">
       <c r="A117" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C117" s="2">
         <v>2782</v>
@@ -2925,10 +2928,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18">
       <c r="A118" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C118" s="2">
         <v>2376</v>
@@ -2939,10 +2942,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18">
       <c r="A119" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C119" s="2">
         <v>2527</v>
@@ -2953,10 +2956,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18">
       <c r="A120" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C120" s="2">
         <v>2757</v>
@@ -2967,10 +2970,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18">
       <c r="A121" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C121" s="2">
         <v>2390</v>
@@ -2981,10 +2984,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18">
       <c r="A122" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C122" s="2">
         <v>2441</v>
@@ -2995,10 +2998,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18">
       <c r="A123" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C123" s="2">
         <v>2524</v>
@@ -3009,10 +3012,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18">
       <c r="A124" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C124" s="2">
         <v>2554</v>
@@ -3023,10 +3026,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18">
       <c r="A125" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C125" s="2">
         <v>2369</v>
@@ -3037,10 +3040,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18">
       <c r="A126" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C126" s="2">
         <v>2806</v>
@@ -3051,10 +3054,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18">
       <c r="A127" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C127" s="2">
         <v>2630</v>
@@ -3065,10 +3068,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18">
       <c r="A128" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C128" s="2">
         <v>2748</v>
@@ -3079,10 +3082,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18">
       <c r="A129" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C129" s="2">
         <v>2442</v>
@@ -3093,10 +3096,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18">
       <c r="A130" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C130" s="2">
         <v>2784</v>
@@ -3107,10 +3110,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18">
       <c r="A131" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C131" s="2">
         <v>2272</v>
@@ -3121,10 +3124,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18">
       <c r="A132" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C132" s="2">
         <v>2359</v>
@@ -3135,10 +3138,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18">
       <c r="A133" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C133" s="2">
         <v>2730</v>
@@ -3149,10 +3152,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18">
       <c r="A134" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C134" s="2">
         <v>2395</v>
@@ -3163,10 +3166,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18">
       <c r="A135" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C135" s="2">
         <v>2389</v>
@@ -3177,10 +3180,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18">
       <c r="A136" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C136" s="2">
         <v>2448</v>
@@ -3191,10 +3194,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18">
       <c r="A137" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C137" s="2">
         <v>2849</v>
@@ -3205,10 +3208,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18">
       <c r="A138" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C138" s="2">
         <v>2818</v>
@@ -3219,10 +3222,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18">
       <c r="A139" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C139" s="2">
         <v>2584</v>
@@ -3233,10 +3236,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18">
       <c r="A140" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C140" s="2">
         <v>2753</v>
@@ -3247,10 +3250,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18">
       <c r="A141" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C141" s="2">
         <v>2325</v>
@@ -3261,10 +3264,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18">
       <c r="A142" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C142" s="2">
         <v>2514</v>
@@ -3275,10 +3278,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18">
       <c r="A143" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C143" s="2">
         <v>2637</v>
@@ -3289,10 +3292,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18">
       <c r="A144" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C144" s="2">
         <v>2423</v>
@@ -3303,10 +3306,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18">
       <c r="A145" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C145" s="2">
         <v>2317</v>
@@ -3317,10 +3320,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18">
       <c r="A146" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C146" s="2">
         <v>2612</v>
@@ -3331,10 +3334,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18">
       <c r="A147" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C147" s="2">
         <v>3751</v>
@@ -3345,10 +3348,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18">
       <c r="A148" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C148" s="2">
         <v>3902</v>
@@ -3359,10 +3362,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18">
       <c r="A149" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C149" s="2">
         <v>2076</v>
@@ -3373,10 +3376,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18">
       <c r="A150" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C150" s="2">
         <v>1897</v>
@@ -3387,10 +3390,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18">
       <c r="A151" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C151" s="2">
         <v>2094</v>
@@ -3401,10 +3404,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18">
       <c r="A152" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C152" s="2">
         <v>2372</v>
@@ -3415,10 +3418,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18">
       <c r="A153" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C153" s="2">
         <v>2186</v>
@@ -3429,10 +3432,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18">
       <c r="A154" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C154" s="2">
         <v>2130</v>
@@ -3443,10 +3446,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18">
       <c r="A155" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C155" s="2">
         <v>2394</v>
@@ -3457,10 +3460,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18">
       <c r="A156" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C156" s="2">
         <v>2017</v>
@@ -3471,10 +3474,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18">
       <c r="A157" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C157" s="2">
         <v>1771</v>
@@ -3485,10 +3488,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18">
       <c r="A158" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C158" s="2">
         <v>1965</v>
@@ -3499,10 +3502,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18">
       <c r="A159" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C159" s="2">
         <v>1749</v>
@@ -3513,10 +3516,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18">
       <c r="A160" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C160" s="2">
         <v>1699</v>
@@ -3527,10 +3530,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18">
       <c r="A161" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C161" s="2">
         <v>1819</v>
@@ -3541,10 +3544,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18">
       <c r="A162" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C162" s="2">
         <v>1751</v>
@@ -3555,10 +3558,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18">
       <c r="A163" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C163" s="2">
         <v>1780</v>
@@ -3569,10 +3572,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18">
       <c r="A164" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C164" s="2">
         <v>1838</v>
@@ -3583,10 +3586,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18">
       <c r="A165" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C165" s="2">
         <v>3032</v>
@@ -3597,10 +3600,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18">
       <c r="A166" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C166" s="2">
         <v>1593</v>
@@ -3611,10 +3614,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18">
       <c r="A167" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C167" s="2">
         <v>5737</v>
@@ -3625,10 +3628,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18">
       <c r="A168" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C168" s="2">
         <v>5314</v>
@@ -3639,10 +3642,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18">
       <c r="A169" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C169" s="2">
         <v>1510</v>
@@ -3653,10 +3656,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18">
       <c r="A170" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C170" s="2">
         <v>2405</v>
@@ -3667,10 +3670,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18">
       <c r="A171" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C171" s="2">
         <v>12964</v>
@@ -3681,10 +3684,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18">
       <c r="A172" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C172" s="2">
         <v>11478</v>
@@ -3695,10 +3698,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18">
       <c r="A173" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C173" s="2">
         <v>12389</v>
@@ -3709,10 +3712,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18">
       <c r="A174" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C174" s="2">
         <v>4337</v>
@@ -3723,10 +3726,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18">
       <c r="A175" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C175" s="2">
         <v>3294</v>
@@ -3737,10 +3740,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18">
       <c r="A176" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C176" s="2">
         <v>1717</v>
@@ -3751,10 +3754,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18">
       <c r="A177" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C177" s="2">
         <v>9602</v>
@@ -3765,10 +3768,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18">
       <c r="A178" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C178" s="2">
         <v>2714</v>
@@ -3779,10 +3782,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18">
       <c r="A179" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C179" s="2">
         <v>2522</v>
@@ -3793,10 +3796,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18">
       <c r="A180" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B180" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="C180" s="2">
         <v>2681</v>
@@ -3807,10 +3810,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18">
       <c r="A181" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C181" s="2">
         <v>2429</v>
@@ -3821,10 +3824,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18">
       <c r="A182" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C182" s="2">
         <v>723</v>
@@ -3835,10 +3838,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="18">
       <c r="A183" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C183" s="2">
         <v>528</v>
@@ -3849,10 +3852,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18">
       <c r="A184" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C184" s="2">
         <v>3060</v>
@@ -3863,10 +3866,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18">
       <c r="A185" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C185" s="2">
         <v>3134</v>
@@ -3877,10 +3880,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18">
       <c r="A186" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C186" s="2">
         <v>3205</v>
@@ -3891,10 +3894,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18">
       <c r="A187" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C187" s="2">
         <v>3153</v>
@@ -3905,10 +3908,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="18">
       <c r="A188" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C188" s="2">
         <v>3012</v>
@@ -3919,10 +3922,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="18">
       <c r="A189" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C189" s="2">
         <v>2907</v>
@@ -3933,10 +3936,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18">
       <c r="A190" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C190" s="2">
         <v>3031</v>
@@ -3947,10 +3950,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18">
       <c r="A191" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C191" s="2">
         <v>4351</v>
@@ -3961,10 +3964,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18">
       <c r="A192" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C192" s="2">
         <v>3675</v>
@@ -3975,10 +3978,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18">
       <c r="A193" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C193" s="2">
         <v>3396</v>
@@ -3989,10 +3992,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="18">
       <c r="A194" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C194" s="2">
         <v>11498</v>
@@ -4003,10 +4006,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="18">
       <c r="A195" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C195" s="2">
         <v>2965</v>
@@ -4017,10 +4020,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="18">
       <c r="A196" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C196" s="2">
         <v>2798</v>
@@ -4031,10 +4034,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="18">
       <c r="A197" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C197" s="2">
         <v>10715</v>
@@ -4045,10 +4048,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="18">
       <c r="A198" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C198" s="2">
         <v>3562</v>
@@ -4059,10 +4062,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="18">
       <c r="A199" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C199" s="2">
         <v>3517</v>
@@ -4073,10 +4076,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="18">
       <c r="A200" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C200" s="2">
         <v>1138</v>
@@ -4087,10 +4090,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="18">
       <c r="A201" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C201" s="2">
         <v>196</v>
@@ -4101,10 +4104,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="18">
       <c r="A202" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C202" s="2">
         <v>273</v>
@@ -4115,10 +4118,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="18">
       <c r="A203" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C203" s="2">
         <v>644</v>
@@ -4129,10 +4132,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="204" customHeight="1" ht="18">
       <c r="A204" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C204" s="2">
         <v>1022</v>
@@ -4143,10 +4146,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="205" customHeight="1" ht="18">
       <c r="A205" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C205" s="2">
         <v>277</v>
@@ -4157,10 +4160,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="206" customHeight="1" ht="18">
       <c r="A206" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C206" s="2">
         <v>40</v>
@@ -4171,10 +4174,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="18">
       <c r="A207" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C207" s="2">
         <v>272</v>
@@ -4185,10 +4188,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="18">
       <c r="A208" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C208" s="2">
         <v>82</v>
@@ -4199,10 +4202,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="209" customHeight="1" ht="18">
       <c r="A209" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C209" s="2">
         <v>295</v>
@@ -4213,10 +4216,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="210" customHeight="1" ht="18">
       <c r="A210" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C210" s="2">
         <v>502</v>
@@ -4227,10 +4230,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="211" customHeight="1" ht="18">
       <c r="A211" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C211" s="2">
         <v>637</v>
@@ -4241,10 +4244,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="212" customHeight="1" ht="18">
       <c r="A212" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C212" s="2">
         <v>443</v>
@@ -4255,10 +4258,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="213" customHeight="1" ht="18">
       <c r="A213" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C213" s="2">
         <v>556</v>
@@ -4269,10 +4272,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="214" customHeight="1" ht="18">
       <c r="A214" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C214" s="2">
         <v>400</v>
@@ -4283,10 +4286,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="215" customHeight="1" ht="18">
       <c r="A215" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C215" s="2">
         <v>568</v>
@@ -4297,10 +4300,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="216" customHeight="1" ht="18">
       <c r="A216" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C216" s="2">
         <v>1045</v>
@@ -4311,10 +4314,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="217" customHeight="1" ht="18">
       <c r="A217" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C217" s="2">
         <v>1009</v>
@@ -4325,10 +4328,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="218" customHeight="1" ht="18">
       <c r="A218" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C218" s="2">
         <v>49</v>
@@ -4339,10 +4342,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="219" customHeight="1" ht="18">
       <c r="A219" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C219" s="2">
         <v>10</v>
@@ -4353,10 +4356,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="220" customHeight="1" ht="18">
       <c r="A220" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C220" s="2">
         <v>5</v>
@@ -4367,10 +4370,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="221" customHeight="1" ht="18">
       <c r="A221" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C221" s="2">
         <v>6</v>
@@ -4381,10 +4384,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="222" customHeight="1" ht="18">
       <c r="A222" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C222" s="2">
         <v>140</v>
@@ -4395,10 +4398,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="223" customHeight="1" ht="18">
       <c r="A223" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C223" s="2">
         <v>34</v>
@@ -4409,10 +4412,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="224" customHeight="1" ht="18">
       <c r="A224" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C224" s="2">
         <v>84</v>
@@ -4423,10 +4426,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="225" customHeight="1" ht="18">
       <c r="A225" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C225" s="2">
         <v>855</v>
@@ -4437,10 +4440,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="226" customHeight="1" ht="18">
       <c r="A226" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C226" s="2">
         <v>513</v>
@@ -4451,10 +4454,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="227" customHeight="1" ht="18">
       <c r="A227" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C227" s="2">
         <v>11800</v>
@@ -4465,10 +4468,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="228" customHeight="1" ht="18">
       <c r="A228" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C228" s="2">
         <v>3268</v>
@@ -4479,10 +4482,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="229" customHeight="1" ht="18">
       <c r="A229" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C229" s="2">
         <v>3673</v>
@@ -4494,8 +4497,8 @@
     <row x14ac:dyDescent="0.25" r="230" customHeight="1" ht="19.5">
       <c r="A230" s="1"/>
       <c r="B230" s="1"/>
-      <c r="C230" s="5"/>
-      <c r="D230" s="5"/>
+      <c r="C230" s="2"/>
+      <c r="D230" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>